<commit_message>
Update DCT analysis scripts and plots; adjust percent recovery calculation and color scheme for improved visualization
</commit_message>
<xml_diff>
--- a/TN066/rip_results.xlsx
+++ b/TN066/rip_results.xlsx
@@ -386,7 +386,7 @@
         </is>
       </c>
       <c r="C2">
-        <v>1.114853021904244</v>
+        <v>111.4853021904244</v>
       </c>
     </row>
     <row r="3">
@@ -401,7 +401,7 @@
         </is>
       </c>
       <c r="C3">
-        <v>0.01489271733354234</v>
+        <v>1.489271733354234</v>
       </c>
     </row>
     <row r="4">
@@ -416,7 +416,7 @@
         </is>
       </c>
       <c r="C4">
-        <v>96.37331703876863</v>
+        <v>9637.331703876864</v>
       </c>
     </row>
     <row r="5">
@@ -431,7 +431,7 @@
         </is>
       </c>
       <c r="C5">
-        <v>0.03823572013580845</v>
+        <v>3.823572013580845</v>
       </c>
     </row>
     <row r="6">
@@ -446,7 +446,7 @@
         </is>
       </c>
       <c r="C6">
-        <v>145.5146425830527</v>
+        <v>14551.46425830527</v>
       </c>
     </row>
     <row r="7">
@@ -461,7 +461,7 @@
         </is>
       </c>
       <c r="C7">
-        <v>0.01852454849342477</v>
+        <v>1.852454849342477</v>
       </c>
     </row>
     <row r="8">
@@ -476,7 +476,7 @@
         </is>
       </c>
       <c r="C8">
-        <v>202.7148577494737</v>
+        <v>20271.48577494737</v>
       </c>
     </row>
     <row r="9">
@@ -491,7 +491,7 @@
         </is>
       </c>
       <c r="C9">
-        <v>18.73520497245247</v>
+        <v>1873.520497245247</v>
       </c>
     </row>
     <row r="10">
@@ -506,7 +506,7 @@
         </is>
       </c>
       <c r="C10">
-        <v>207.3278129825612</v>
+        <v>20732.78129825612</v>
       </c>
     </row>
     <row r="11">
@@ -521,7 +521,7 @@
         </is>
       </c>
       <c r="C11">
-        <v>0.04897177131845247</v>
+        <v>4.897177131845247</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor enrichment calculations and update plots; replace percent recovery with enrichment metrics and adjust plot titles and file names for clarity
</commit_message>
<xml_diff>
--- a/TN066/rip_results.xlsx
+++ b/TN066/rip_results.xlsx
@@ -370,7 +370,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>percent_recovery</t>
+          <t>enrichment</t>
         </is>
       </c>
     </row>
@@ -386,7 +386,7 @@
         </is>
       </c>
       <c r="C2">
-        <v>111.4853021904244</v>
+        <v>1.114853021904244</v>
       </c>
     </row>
     <row r="3">
@@ -401,7 +401,7 @@
         </is>
       </c>
       <c r="C3">
-        <v>1.489271733354234</v>
+        <v>0.01489271733354234</v>
       </c>
     </row>
     <row r="4">
@@ -416,7 +416,7 @@
         </is>
       </c>
       <c r="C4">
-        <v>9637.331703876864</v>
+        <v>96.37331703876863</v>
       </c>
     </row>
     <row r="5">
@@ -431,7 +431,7 @@
         </is>
       </c>
       <c r="C5">
-        <v>3.823572013580845</v>
+        <v>0.03823572013580845</v>
       </c>
     </row>
     <row r="6">
@@ -446,7 +446,7 @@
         </is>
       </c>
       <c r="C6">
-        <v>14551.46425830527</v>
+        <v>145.5146425830527</v>
       </c>
     </row>
     <row r="7">
@@ -461,7 +461,7 @@
         </is>
       </c>
       <c r="C7">
-        <v>1.852454849342477</v>
+        <v>0.01852454849342477</v>
       </c>
     </row>
     <row r="8">
@@ -476,7 +476,7 @@
         </is>
       </c>
       <c r="C8">
-        <v>20271.48577494737</v>
+        <v>202.7148577494737</v>
       </c>
     </row>
     <row r="9">
@@ -491,7 +491,7 @@
         </is>
       </c>
       <c r="C9">
-        <v>1873.520497245247</v>
+        <v>18.73520497245247</v>
       </c>
     </row>
     <row r="10">
@@ -506,7 +506,7 @@
         </is>
       </c>
       <c r="C10">
-        <v>20732.78129825612</v>
+        <v>207.3278129825612</v>
       </c>
     </row>
     <row r="11">
@@ -521,7 +521,7 @@
         </is>
       </c>
       <c r="C11">
-        <v>4.897177131845247</v>
+        <v>0.04897177131845247</v>
       </c>
     </row>
   </sheetData>

</xml_diff>